<commit_message>
gecko issue solved - 3rd Commit
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="9810" windowHeight="5580"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11625" windowHeight="4980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,19 +33,19 @@
     <t>InitialBalance</t>
   </si>
   <si>
+    <t>Test Homelone</t>
+  </si>
+  <si>
+    <t>Buying House</t>
+  </si>
+  <si>
     <t>techfiosdemo@gmail.com</t>
   </si>
   <si>
     <t>abc123</t>
   </si>
   <si>
-    <t>Test Homelone</t>
-  </si>
-  <si>
-    <t>Buying House</t>
-  </si>
-  <si>
-    <t>BrowserName</t>
+    <t>BrowseName</t>
   </si>
   <si>
     <t>firefox</t>
@@ -398,23 +398,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -425,15 +425,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -441,6 +441,7 @@
     <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -471,10 +472,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>10000</v>

</xml_diff>

<commit_message>
DDFXSSF - 4th Commit
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11625" windowHeight="4980"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14220" windowHeight="4140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K17"/>
+  <oleSize ref="A1:J12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>UserName</t>
   </si>
@@ -48,7 +48,10 @@
     <t>BrowseName</t>
   </si>
   <si>
-    <t>firefox</t>
+    <t>a1000</t>
+  </si>
+  <si>
+    <t>chrome</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +430,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -450,7 +453,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,8 +480,8 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>10000</v>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>